<commit_message>
update keras model 1280 and 2560
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">ACC</t>
   </si>
@@ -40,16 +40,16 @@
     <t xml:space="preserve">Paper (Ori)</t>
   </si>
   <si>
-    <t xml:space="preserve">Paper (rerun)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MiniInceptionTime (keras)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MiniInceptionTime (pytorch)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x</t>
+    <t xml:space="preserve">Paper (rerun – pytorch)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paper (rerun – keras)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MiniInceptionTime (keras – 2560)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MiniInceptionTime (keras – 1280)</t>
   </si>
 </sst>
 </file>
@@ -64,6 +64,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -85,6 +86,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -163,15 +165,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.84"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -236,39 +238,59 @@
         <v>7</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>98.97</v>
+        <v>98.85</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>98.97</v>
+        <v>98.85</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>99.45</v>
+        <v>99.43</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>98.96</v>
+        <v>98.83</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>6261</v>
+        <v>11065</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="3" t="n">
+        <v>98.97</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>98.97</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>99.45</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>98.96</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>6261</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>9</v>
+      <c r="B6" s="3" t="n">
+        <v>98.85</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>98.85</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>99.39</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>98.83</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>6261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>